<commit_message>
Add condition and more event 1
</commit_message>
<xml_diff>
--- a/DataSource/excel/condition.xlsx
+++ b/DataSource/excel/condition.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8120" yWindow="1000" windowWidth="25120" windowHeight="14400" tabRatio="500"/>
+    <workbookView xWindow="7440" yWindow="2240" windowWidth="25120" windowHeight="14400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="condition.csv" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>id</t>
   </si>
@@ -59,21 +59,12 @@
     <t>没有签约</t>
   </si>
   <si>
-    <t>currCityPercent</t>
-  </si>
-  <si>
-    <t>=</t>
-  </si>
-  <si>
     <t>haveRecommendLetter</t>
   </si>
   <si>
     <t>有推荐信</t>
   </si>
   <si>
-    <t>haveItem</t>
-  </si>
-  <si>
     <t>;</t>
   </si>
   <si>
@@ -83,7 +74,25 @@
     <t>可以传播谣言</t>
   </si>
   <si>
-    <t>hasJob</t>
+    <t>subtype</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>percentage</t>
+  </si>
+  <si>
+    <t>item</t>
+  </si>
+  <si>
+    <t>job</t>
+  </si>
+  <si>
+    <t>guild</t>
+  </si>
+  <si>
+    <t>&lt;=</t>
   </si>
 </sst>
 </file>
@@ -494,21 +503,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="15.1640625" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -519,13 +528,16 @@
         <v>6</v>
       </c>
       <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -541,8 +553,11 @@
       <c r="E2" t="s">
         <v>3</v>
       </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -550,47 +565,56 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3">
-        <v>0</v>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4">
+        <v>209</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
+      <c r="F5">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Continue to set separate functions (for government)
</commit_message>
<xml_diff>
--- a/DataSource/excel/condition.xlsx
+++ b/DataSource/excel/condition.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7440" yWindow="2240" windowWidth="25120" windowHeight="14400" tabRatio="500"/>
+    <workbookView xWindow="7440" yWindow="1340" windowWidth="25120" windowHeight="14400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="condition.csv" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
   <si>
     <t>id</t>
   </si>
@@ -59,6 +59,9 @@
     <t>没有签约</t>
   </si>
   <si>
+    <t>=</t>
+  </si>
+  <si>
     <t>haveRecommendLetter</t>
   </si>
   <si>
@@ -93,6 +96,60 @@
   </si>
   <si>
     <t>&lt;=</t>
+  </si>
+  <si>
+    <t>canSignUp</t>
+  </si>
+  <si>
+    <t>是否可以签约</t>
+  </si>
+  <si>
+    <t>totalPercentage</t>
+  </si>
+  <si>
+    <t>&lt;</t>
+  </si>
+  <si>
+    <t>canSignUp1</t>
+  </si>
+  <si>
+    <t>canSignUp2</t>
+  </si>
+  <si>
+    <t>guildNumber</t>
+  </si>
+  <si>
+    <t>是否可以签约条件1</t>
+  </si>
+  <si>
+    <t>是否可以签约条件2</t>
+  </si>
+  <si>
+    <t>and</t>
+  </si>
+  <si>
+    <t>canSignUp1;canSignUp2</t>
+  </si>
+  <si>
+    <t>canSignUpMoneyEnough</t>
+  </si>
+  <si>
+    <t>签约金够</t>
+  </si>
+  <si>
+    <t>money</t>
+  </si>
+  <si>
+    <t>signUpMoney</t>
+  </si>
+  <si>
+    <t>canMilitaryInvestMoneyEnough</t>
+  </si>
+  <si>
+    <t>军事投资钱是否够</t>
+  </si>
+  <si>
+    <t>militaryInvestMoney</t>
   </si>
 </sst>
 </file>
@@ -503,18 +560,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="15.1640625" customWidth="1"/>
     <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -528,7 +586,7 @@
         <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E1" t="s">
         <v>7</v>
@@ -565,33 +623,33 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="F3">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F4">
         <v>209</v>
@@ -599,22 +657,122 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
         <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" t="s">
-        <v>12</v>
       </c>
       <c r="F5">
         <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Continue to change structure
</commit_message>
<xml_diff>
--- a/DataSource/excel/condition.xlsx
+++ b/DataSource/excel/condition.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12600" yWindow="1460" windowWidth="25120" windowHeight="14400" tabRatio="500"/>
+    <workbookView xWindow="3680" yWindow="1280" windowWidth="25120" windowHeight="14400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="condition.csv" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="71">
   <si>
     <t>id</t>
   </si>
@@ -210,6 +210,36 @@
   </si>
   <si>
     <t>钱够</t>
+  </si>
+  <si>
+    <t>canCommerceInvestMoneyEnough</t>
+  </si>
+  <si>
+    <t>商业投资钱是否够</t>
+  </si>
+  <si>
+    <t>commerceInvestMoney</t>
+  </si>
+  <si>
+    <t>tradeCondition</t>
+  </si>
+  <si>
+    <t>签约了</t>
+  </si>
+  <si>
+    <t>canUnblockTradeItem</t>
+  </si>
+  <si>
+    <t>可以解锁商品</t>
+  </si>
+  <si>
+    <t>cacheString</t>
+  </si>
+  <si>
+    <t>tradeUnblockItem</t>
+  </si>
+  <si>
+    <t>!=</t>
   </si>
 </sst>
 </file>
@@ -620,17 +650,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="15.1640625" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="22.1640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -980,6 +1011,75 @@
         <v>35</v>
       </c>
     </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
continue to make structure change
</commit_message>
<xml_diff>
--- a/DataSource/excel/condition.xlsx
+++ b/DataSource/excel/condition.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3680" yWindow="1280" windowWidth="25120" windowHeight="14400" tabRatio="500"/>
+    <workbookView xWindow="26080" yWindow="4100" windowWidth="25120" windowHeight="14400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="condition.csv" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="82">
   <si>
     <t>id</t>
   </si>
@@ -158,9 +158,6 @@
     <t>是否有船</t>
   </si>
   <si>
-    <t>hireSailorHaveShip</t>
-  </si>
-  <si>
     <t>ship</t>
   </si>
   <si>
@@ -206,9 +203,6 @@
     <t>needNumber</t>
   </si>
   <si>
-    <t>hireSailorMoneyEnough</t>
-  </si>
-  <si>
     <t>钱够</t>
   </si>
   <si>
@@ -240,6 +234,45 @@
   </si>
   <si>
     <t>!=</t>
+  </si>
+  <si>
+    <t>haveShip</t>
+  </si>
+  <si>
+    <t>shipNumberExceed</t>
+  </si>
+  <si>
+    <t>船只满了</t>
+  </si>
+  <si>
+    <t>haveShip2Sell</t>
+  </si>
+  <si>
+    <t>shipNumber</t>
+  </si>
+  <si>
+    <t>haveShipInDock</t>
+  </si>
+  <si>
+    <t>船坞有船</t>
+  </si>
+  <si>
+    <t>是否有船可卖</t>
+  </si>
+  <si>
+    <t>or</t>
+  </si>
+  <si>
+    <t>haveShipInDock;have2Ship</t>
+  </si>
+  <si>
+    <t>have2Ship</t>
+  </si>
+  <si>
+    <t>有至少两只船</t>
+  </si>
+  <si>
+    <t>moneyEnough</t>
   </si>
 </sst>
 </file>
@@ -650,10 +683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -683,10 +716,10 @@
         <v>6</v>
       </c>
       <c r="F1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -729,7 +762,7 @@
         <v>9</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -752,7 +785,7 @@
         <v>12</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G4">
         <v>209</v>
@@ -775,7 +808,7 @@
         <v>12</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G5">
         <v>12</v>
@@ -798,7 +831,7 @@
         <v>25</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G6">
         <v>100</v>
@@ -821,7 +854,7 @@
         <v>25</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G7">
         <v>3</v>
@@ -898,22 +931,22 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="B11" t="s">
         <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E11" t="s">
         <v>36</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -921,45 +954,45 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" t="s">
         <v>46</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" t="s">
         <v>47</v>
-      </c>
-      <c r="C12" t="s">
-        <v>51</v>
-      </c>
-      <c r="D12" t="s">
-        <v>48</v>
       </c>
       <c r="E12" t="s">
         <v>37</v>
       </c>
       <c r="F12" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" t="s">
         <v>51</v>
-      </c>
-      <c r="G12" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" t="s">
         <v>53</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" t="s">
         <v>54</v>
-      </c>
-      <c r="C13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" t="s">
-        <v>55</v>
       </c>
       <c r="E13" t="s">
         <v>36</v>
       </c>
       <c r="F13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G13">
         <v>0</v>
@@ -967,33 +1000,33 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" t="s">
         <v>56</v>
       </c>
-      <c r="B14" t="s">
-        <v>57</v>
-      </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E14" t="s">
         <v>37</v>
       </c>
       <c r="F14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C15" t="s">
         <v>20</v>
@@ -1005,7 +1038,7 @@
         <v>37</v>
       </c>
       <c r="F15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G15" t="s">
         <v>35</v>
@@ -1013,16 +1046,16 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C16" t="s">
         <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E16" t="s">
         <v>21</v>
@@ -1036,10 +1069,10 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C17" t="s">
         <v>16</v>
@@ -1051,7 +1084,7 @@
         <v>36</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -1059,24 +1092,116 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" t="s">
         <v>66</v>
       </c>
-      <c r="B18" t="s">
+      <c r="D18" t="s">
         <v>67</v>
       </c>
-      <c r="C18" t="s">
+      <c r="E18" t="s">
         <v>68</v>
       </c>
-      <c r="D18" t="s">
-        <v>69</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
+        <v>44</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>70</v>
       </c>
-      <c r="F18" t="s">
-        <v>45</v>
-      </c>
-      <c r="G18">
+      <c r="B19" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" t="s">
+        <v>44</v>
+      </c>
+      <c r="G19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" t="s">
+        <v>76</v>
+      </c>
+      <c r="C20" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" t="s">
+        <v>78</v>
+      </c>
+      <c r="G20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>79</v>
+      </c>
+      <c r="B21" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" t="s">
+        <v>36</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" t="s">
+        <v>73</v>
+      </c>
+      <c r="E22" t="s">
+        <v>36</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G22">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
structure change continue -- doing item browse part
</commit_message>
<xml_diff>
--- a/DataSource/excel/condition.xlsx
+++ b/DataSource/excel/condition.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="85">
   <si>
     <t>id</t>
   </si>
@@ -273,6 +273,15 @@
   </si>
   <si>
     <t>moneyEnough</t>
+  </si>
+  <si>
+    <t>cityHaveItem</t>
+  </si>
+  <si>
+    <t>城市有道具卖</t>
+  </si>
+  <si>
+    <t>sellItemNumber</t>
   </si>
 </sst>
 </file>
@@ -683,10 +692,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1205,6 +1214,29 @@
         <v>0</v>
       </c>
     </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>82</v>
+      </c>
+      <c r="B23" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" t="s">
+        <v>84</v>
+      </c>
+      <c r="E23" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23" t="s">
+        <v>44</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Change data structure, finish shop buy/sell
</commit_message>
<xml_diff>
--- a/DataSource/excel/condition.xlsx
+++ b/DataSource/excel/condition.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="26080" yWindow="4100" windowWidth="25120" windowHeight="14400" tabRatio="500"/>
+    <workbookView xWindow="21320" yWindow="4760" windowWidth="25120" windowHeight="14400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="condition.csv" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="87">
   <si>
     <t>id</t>
   </si>
@@ -282,6 +282,12 @@
   </si>
   <si>
     <t>sellItemNumber</t>
+  </si>
+  <si>
+    <t>有可出售道具</t>
+  </si>
+  <si>
+    <t>haveItem</t>
   </si>
 </sst>
 </file>
@@ -692,10 +698,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1237,6 +1243,29 @@
         <v>0</v>
       </c>
     </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>86</v>
+      </c>
+      <c r="B24" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" t="s">
+        <v>84</v>
+      </c>
+      <c r="E24" t="s">
+        <v>36</v>
+      </c>
+      <c r="F24" t="s">
+        <v>44</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
change the observer type, --to be continue
</commit_message>
<xml_diff>
--- a/DataSource/excel/condition.xlsx
+++ b/DataSource/excel/condition.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="90">
   <si>
     <t>id</t>
   </si>
@@ -288,6 +288,15 @@
   </si>
   <si>
     <t>haveItem</t>
+  </si>
+  <si>
+    <t>itemCanEquip</t>
+  </si>
+  <si>
+    <t>道具可以装备</t>
+  </si>
+  <si>
+    <t>category</t>
   </si>
 </sst>
 </file>
@@ -698,10 +707,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1266,6 +1275,29 @@
         <v>0</v>
       </c>
     </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>87</v>
+      </c>
+      <c r="B25" t="s">
+        <v>88</v>
+      </c>
+      <c r="C25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" t="s">
+        <v>89</v>
+      </c>
+      <c r="E25" t="s">
+        <v>21</v>
+      </c>
+      <c r="F25" t="s">
+        <v>44</v>
+      </c>
+      <c r="G25">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
clean the code, remove listener. finish window related
</commit_message>
<xml_diff>
--- a/DataSource/excel/condition.xlsx
+++ b/DataSource/excel/condition.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="98">
   <si>
     <t>id</t>
   </si>
@@ -297,6 +297,30 @@
   </si>
   <si>
     <t>category</t>
+  </si>
+  <si>
+    <t>itemCanEquipToRole</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>某角色可以装备</t>
+  </si>
+  <si>
+    <t>itemAlreadyEquiped</t>
+  </si>
+  <si>
+    <t>已经装备上了</t>
+  </si>
+  <si>
+    <t>isEquiped</t>
+  </si>
+  <si>
+    <t>canEquip:</t>
   </si>
 </sst>
 </file>
@@ -707,10 +731,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1298,6 +1322,52 @@
         <v>3</v>
       </c>
     </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>90</v>
+      </c>
+      <c r="B26" t="s">
+        <v>93</v>
+      </c>
+      <c r="C26" t="s">
+        <v>92</v>
+      </c>
+      <c r="D26" t="s">
+        <v>91</v>
+      </c>
+      <c r="E26" t="s">
+        <v>97</v>
+      </c>
+      <c r="F26" t="s">
+        <v>92</v>
+      </c>
+      <c r="G26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>94</v>
+      </c>
+      <c r="B27" t="s">
+        <v>95</v>
+      </c>
+      <c r="C27" t="s">
+        <v>92</v>
+      </c>
+      <c r="D27" t="s">
+        <v>18</v>
+      </c>
+      <c r="E27" t="s">
+        <v>96</v>
+      </c>
+      <c r="F27" t="s">
+        <v>12</v>
+      </c>
+      <c r="G27" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
add shipheader equip part 1
</commit_message>
<xml_diff>
--- a/DataSource/excel/condition.xlsx
+++ b/DataSource/excel/condition.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="104">
   <si>
     <t>id</t>
   </si>
@@ -321,6 +321,24 @@
   </si>
   <si>
     <t>canEquip:</t>
+  </si>
+  <si>
+    <t>itemNotNil</t>
+  </si>
+  <si>
+    <t>选择了装备</t>
+  </si>
+  <si>
+    <t>nil</t>
+  </si>
+  <si>
+    <t>shipHasHeader</t>
+  </si>
+  <si>
+    <t>装备了船首像</t>
+  </si>
+  <si>
+    <t>shipHeader</t>
   </si>
 </sst>
 </file>
@@ -731,10 +749,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1368,6 +1386,49 @@
         <v>12</v>
       </c>
     </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>98</v>
+      </c>
+      <c r="B28" t="s">
+        <v>99</v>
+      </c>
+      <c r="C28" t="s">
+        <v>92</v>
+      </c>
+      <c r="D28" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28" t="s">
+        <v>68</v>
+      </c>
+      <c r="F28" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>101</v>
+      </c>
+      <c r="B29" t="s">
+        <v>102</v>
+      </c>
+      <c r="C29" t="s">
+        <v>92</v>
+      </c>
+      <c r="D29" t="s">
+        <v>43</v>
+      </c>
+      <c r="E29" t="s">
+        <v>103</v>
+      </c>
+      <c r="F29" t="s">
+        <v>12</v>
+      </c>
+      <c r="G29" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Add equip ship from item
</commit_message>
<xml_diff>
--- a/DataSource/excel/condition.xlsx
+++ b/DataSource/excel/condition.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="54660" yWindow="7900" windowWidth="25120" windowHeight="14400" tabRatio="500"/>
+    <workbookView xWindow="49340" yWindow="8300" windowWidth="25120" windowHeight="14400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="condition.csv" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="106">
   <si>
     <t>id</t>
   </si>
@@ -339,6 +339,12 @@
   </si>
   <si>
     <t>shipHeader</t>
+  </si>
+  <si>
+    <t>itemIsShipHeader</t>
+  </si>
+  <si>
+    <t>是否是船首像</t>
   </si>
 </sst>
 </file>
@@ -749,10 +755,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1429,6 +1435,29 @@
         <v>12</v>
       </c>
     </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>104</v>
+      </c>
+      <c r="B30" t="s">
+        <v>105</v>
+      </c>
+      <c r="C30" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" t="s">
+        <v>5</v>
+      </c>
+      <c r="E30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" t="s">
+        <v>44</v>
+      </c>
+      <c r="G30">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Add sail related and base data
</commit_message>
<xml_diff>
--- a/DataSource/excel/condition.xlsx
+++ b/DataSource/excel/condition.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="49340" yWindow="8300" windowWidth="25120" windowHeight="14400" tabRatio="500"/>
+    <workbookView xWindow="50060" yWindow="10020" windowWidth="20620" windowHeight="20220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="condition.csv" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="117">
   <si>
     <t>id</t>
   </si>
@@ -143,18 +143,12 @@
     <t>&gt;=</t>
   </si>
   <si>
-    <t>signUpMoney</t>
-  </si>
-  <si>
     <t>canMilitaryInvestMoneyEnough</t>
   </si>
   <si>
     <t>军事投资钱是否够</t>
   </si>
   <si>
-    <t>militaryInvestMoney</t>
-  </si>
-  <si>
     <t>是否有船</t>
   </si>
   <si>
@@ -212,9 +206,6 @@
     <t>商业投资钱是否够</t>
   </si>
   <si>
-    <t>commerceInvestMoney</t>
-  </si>
-  <si>
     <t>tradeCondition</t>
   </si>
   <si>
@@ -345,6 +336,48 @@
   </si>
   <si>
     <t>是否是船首像</t>
+  </si>
+  <si>
+    <t>haveSailors</t>
+  </si>
+  <si>
+    <t>是否有船员</t>
+  </si>
+  <si>
+    <t>team</t>
+  </si>
+  <si>
+    <t>haveEnoughSailors</t>
+  </si>
+  <si>
+    <t>船员达到必要数</t>
+  </si>
+  <si>
+    <t>needFillUp</t>
+  </si>
+  <si>
+    <t>需要不急</t>
+  </si>
+  <si>
+    <t>needsFoodCapacity</t>
+  </si>
+  <si>
+    <t>sailDaysEnough</t>
+  </si>
+  <si>
+    <t>航行天数是否足够</t>
+  </si>
+  <si>
+    <t>days</t>
+  </si>
+  <si>
+    <t>signUpUnitValue</t>
+  </si>
+  <si>
+    <t>milltaryValue</t>
+  </si>
+  <si>
+    <t>commerceValue</t>
   </si>
 </sst>
 </file>
@@ -755,10 +788,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -788,10 +821,10 @@
         <v>6</v>
       </c>
       <c r="F1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -834,7 +867,7 @@
         <v>9</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -848,19 +881,19 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G4">
-        <v>209</v>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -880,7 +913,7 @@
         <v>12</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G5">
         <v>12</v>
@@ -903,7 +936,7 @@
         <v>25</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G6">
         <v>100</v>
@@ -926,7 +959,7 @@
         <v>25</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G7">
         <v>3</v>
@@ -966,7 +999,7 @@
         <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>114</v>
       </c>
       <c r="E9" t="s">
         <v>21</v>
@@ -980,16 +1013,16 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s">
         <v>39</v>
-      </c>
-      <c r="B10" t="s">
-        <v>40</v>
       </c>
       <c r="C10" t="s">
         <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
+        <v>115</v>
       </c>
       <c r="E10" t="s">
         <v>21</v>
@@ -1003,22 +1036,22 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>105</v>
       </c>
       <c r="D11" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="E11" t="s">
         <v>36</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -1026,45 +1059,45 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" t="s">
         <v>45</v>
-      </c>
-      <c r="B12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" t="s">
-        <v>47</v>
       </c>
       <c r="E12" t="s">
         <v>37</v>
       </c>
       <c r="F12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" t="s">
         <v>52</v>
-      </c>
-      <c r="B13" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" t="s">
-        <v>50</v>
-      </c>
-      <c r="D13" t="s">
-        <v>54</v>
       </c>
       <c r="E13" t="s">
         <v>36</v>
       </c>
       <c r="F13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G13">
         <v>0</v>
@@ -1072,33 +1105,33 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E14" t="s">
         <v>37</v>
       </c>
       <c r="F14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C15" t="s">
         <v>20</v>
@@ -1110,7 +1143,7 @@
         <v>37</v>
       </c>
       <c r="F15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G15" t="s">
         <v>35</v>
@@ -1118,16 +1151,16 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C16" t="s">
         <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>61</v>
+        <v>116</v>
       </c>
       <c r="E16" t="s">
         <v>21</v>
@@ -1141,10 +1174,10 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B17" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C17" t="s">
         <v>16</v>
@@ -1156,7 +1189,7 @@
         <v>36</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -1164,22 +1197,22 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" t="s">
         <v>64</v>
       </c>
-      <c r="B18" t="s">
+      <c r="E18" t="s">
         <v>65</v>
       </c>
-      <c r="C18" t="s">
-        <v>66</v>
-      </c>
-      <c r="D18" t="s">
-        <v>67</v>
-      </c>
-      <c r="E18" t="s">
-        <v>68</v>
-      </c>
       <c r="F18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -1187,22 +1220,22 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" t="s">
+        <v>105</v>
+      </c>
+      <c r="D19" t="s">
         <v>70</v>
-      </c>
-      <c r="B19" t="s">
-        <v>71</v>
-      </c>
-      <c r="C19" t="s">
-        <v>43</v>
-      </c>
-      <c r="D19" t="s">
-        <v>44</v>
       </c>
       <c r="E19" t="s">
         <v>37</v>
       </c>
       <c r="F19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G19">
         <v>5</v>
@@ -1210,13 +1243,13 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B20" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C20" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D20" t="s">
         <v>12</v>
@@ -1225,7 +1258,7 @@
         <v>12</v>
       </c>
       <c r="F20" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G20" t="s">
         <v>12</v>
@@ -1233,22 +1266,22 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B21" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C21" t="s">
-        <v>43</v>
+        <v>105</v>
       </c>
       <c r="D21" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="E21" t="s">
         <v>36</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -1256,22 +1289,22 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B22" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C22" t="s">
         <v>16</v>
       </c>
       <c r="D22" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E22" t="s">
         <v>36</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -1279,22 +1312,22 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B23" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C23" t="s">
         <v>16</v>
       </c>
       <c r="D23" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E23" t="s">
         <v>36</v>
       </c>
       <c r="F23" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G23">
         <v>0</v>
@@ -1302,22 +1335,22 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B24" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C24" t="s">
         <v>20</v>
       </c>
       <c r="D24" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E24" t="s">
         <v>36</v>
       </c>
       <c r="F24" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G24">
         <v>0</v>
@@ -1325,22 +1358,22 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B25" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C25" t="s">
         <v>18</v>
       </c>
       <c r="D25" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E25" t="s">
         <v>21</v>
       </c>
       <c r="F25" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G25">
         <v>3</v>
@@ -1348,22 +1381,22 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>87</v>
+      </c>
+      <c r="B26" t="s">
         <v>90</v>
       </c>
-      <c r="B26" t="s">
-        <v>93</v>
-      </c>
       <c r="C26" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D26" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E26" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F26" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G26" t="s">
         <v>18</v>
@@ -1371,19 +1404,19 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B27" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C27" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D27" t="s">
         <v>18</v>
       </c>
       <c r="E27" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F27" t="s">
         <v>12</v>
@@ -1394,39 +1427,39 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B28" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C28" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D28" t="s">
         <v>18</v>
       </c>
       <c r="E28" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F28" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B29" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C29" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D29" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E29" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F29" t="s">
         <v>12</v>
@@ -1437,10 +1470,10 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B30" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C30" t="s">
         <v>18</v>
@@ -1452,10 +1485,102 @@
         <v>9</v>
       </c>
       <c r="F30" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G30">
         <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>103</v>
+      </c>
+      <c r="B31" t="s">
+        <v>104</v>
+      </c>
+      <c r="C31" t="s">
+        <v>105</v>
+      </c>
+      <c r="D31" t="s">
+        <v>103</v>
+      </c>
+      <c r="E31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" t="s">
+        <v>42</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>106</v>
+      </c>
+      <c r="B32" t="s">
+        <v>107</v>
+      </c>
+      <c r="C32" t="s">
+        <v>105</v>
+      </c>
+      <c r="D32" t="s">
+        <v>106</v>
+      </c>
+      <c r="E32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" t="s">
+        <v>42</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>108</v>
+      </c>
+      <c r="B33" t="s">
+        <v>109</v>
+      </c>
+      <c r="C33" t="s">
+        <v>105</v>
+      </c>
+      <c r="D33" t="s">
+        <v>110</v>
+      </c>
+      <c r="E33" t="s">
+        <v>36</v>
+      </c>
+      <c r="F33" t="s">
+        <v>42</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>111</v>
+      </c>
+      <c r="B34" t="s">
+        <v>112</v>
+      </c>
+      <c r="C34" t="s">
+        <v>48</v>
+      </c>
+      <c r="D34" t="s">
+        <v>113</v>
+      </c>
+      <c r="E34" t="s">
+        <v>36</v>
+      </c>
+      <c r="F34" t="s">
+        <v>42</v>
+      </c>
+      <c r="G34">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1. Add tasks (part of it) 2. Fix main menu bug
</commit_message>
<xml_diff>
--- a/DataSource/excel/condition.xlsx
+++ b/DataSource/excel/condition.xlsx
@@ -1,33 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27610"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yujiel/Documents/mygit/SailingGame/DataSource/excel/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="50060" yWindow="10020" windowWidth="20620" windowHeight="20220" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14640" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="condition.csv" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="120">
   <si>
     <t>id</t>
   </si>
@@ -378,6 +373,15 @@
   </si>
   <si>
     <t>commerceValue</t>
+  </si>
+  <si>
+    <t>cityHasTasks</t>
+  </si>
+  <si>
+    <t>城市是否有任务</t>
+  </si>
+  <si>
+    <t>taskNumber</t>
   </si>
 </sst>
 </file>
@@ -390,6 +394,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -788,13 +793,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="29.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1"/>
@@ -804,7 +809,7 @@
     <col min="6" max="7" width="22.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -827,7 +832,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -850,7 +855,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -873,7 +878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -896,7 +901,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -919,7 +924,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
@@ -942,7 +947,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
@@ -965,7 +970,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -988,7 +993,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
         <v>33</v>
       </c>
@@ -1011,7 +1016,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -1034,7 +1039,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
         <v>66</v>
       </c>
@@ -1057,7 +1062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -1080,7 +1085,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -1103,7 +1108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>53</v>
       </c>
@@ -1126,7 +1131,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>78</v>
       </c>
@@ -1149,7 +1154,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>57</v>
       </c>
@@ -1172,7 +1177,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>59</v>
       </c>
@@ -1195,7 +1200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>61</v>
       </c>
@@ -1218,7 +1223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>67</v>
       </c>
@@ -1241,7 +1246,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>69</v>
       </c>
@@ -1264,7 +1269,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>76</v>
       </c>
@@ -1287,7 +1292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>71</v>
       </c>
@@ -1310,7 +1315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>79</v>
       </c>
@@ -1333,7 +1338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>83</v>
       </c>
@@ -1356,7 +1361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>84</v>
       </c>
@@ -1379,7 +1384,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>87</v>
       </c>
@@ -1402,7 +1407,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>91</v>
       </c>
@@ -1425,7 +1430,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>95</v>
       </c>
@@ -1445,7 +1450,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>98</v>
       </c>
@@ -1468,7 +1473,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
         <v>101</v>
       </c>
@@ -1491,7 +1496,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
         <v>103</v>
       </c>
@@ -1514,7 +1519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
         <v>106</v>
       </c>
@@ -1537,7 +1542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
         <v>108</v>
       </c>
@@ -1560,7 +1565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7">
       <c r="A34" t="s">
         <v>111</v>
       </c>
@@ -1581,10 +1586,38 @@
       </c>
       <c r="G34">
         <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" t="s">
+        <v>117</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C35" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" t="s">
+        <v>119</v>
+      </c>
+      <c r="E35" t="s">
+        <v>36</v>
+      </c>
+      <c r="F35" t="s">
+        <v>42</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix bunches of bugs
</commit_message>
<xml_diff>
--- a/DataSource/excel/condition.xlsx
+++ b/DataSource/excel/condition.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8100" yWindow="840" windowWidth="25360" windowHeight="14640" tabRatio="500"/>
+    <workbookView xWindow="8000" yWindow="840" windowWidth="25360" windowHeight="14640" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="condition.csv" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="128">
   <si>
     <t>id</t>
   </si>
@@ -402,6 +402,15 @@
   </si>
   <si>
     <t>玩家没有任务</t>
+  </si>
+  <si>
+    <t>isSailFlagYes</t>
+  </si>
+  <si>
+    <t>是否出海</t>
+  </si>
+  <si>
+    <t>sailFlag</t>
   </si>
 </sst>
 </file>
@@ -812,10 +821,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1676,6 +1685,29 @@
         <v>12</v>
       </c>
     </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>125</v>
+      </c>
+      <c r="B38" t="s">
+        <v>126</v>
+      </c>
+      <c r="C38" t="s">
+        <v>48</v>
+      </c>
+      <c r="D38" t="s">
+        <v>127</v>
+      </c>
+      <c r="E38" t="s">
+        <v>65</v>
+      </c>
+      <c r="F38" t="s">
+        <v>42</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Continue working on task
</commit_message>
<xml_diff>
--- a/DataSource/excel/condition.xlsx
+++ b/DataSource/excel/condition.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8000" yWindow="840" windowWidth="25360" windowHeight="14640" tabRatio="500"/>
+    <workbookView xWindow="3440" yWindow="840" windowWidth="25360" windowHeight="14640" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="condition.csv" sheetId="1" r:id="rId1"/>
@@ -823,8 +823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>